<commit_message>
separate Annex 2 in a dedicated document
</commit_message>
<xml_diff>
--- a/tools/anssi/secnumcloud-3.2.xlsx
+++ b/tools/anssi/secnumcloud-3.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/anssi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FBA173-476E-1249-A097-82F615F20B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EA5330-2E8C-9841-B014-F34E873B4332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" activeTab="1" xr2:uid="{125C4C37-F3C0-444B-A950-381456F8AB10}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="1148">
   <si>
     <t>description</t>
   </si>
@@ -3665,18 +3665,6 @@
     <t xml:space="preserve">Recommandations pour les entreprises qui envisagent de souscrire à des services de cloud computing. </t>
   </si>
   <si>
-    <t>Cette annexe liste les recommandations de l’ANSSI aux commanditaires de prestations d’informatique en nuage.</t>
-  </si>
-  <si>
-    <t>En effet, un prestataire qualifié garde la faculté de réaliser des prestations non qualifiées. Le recours à un prestataire issu du catalogue des prestataires qualifiés est donc une condition nécessaire mais pas suffisante pour bénéficier d’une prestation qualifiée, le commanditaire doit donc également exiger une prestation qualifiée.</t>
-  </si>
-  <si>
-    <t>S’il s’avère après instruction de la réclamation que le prestataire n’a pas respecté une ou plusieurs exigences du présent référentiel dans le cadre d’une prestation qualifiée, et selon la gravité, la qualification du prestataire peut être suspendue, retirée ou sa portée de qualification réduite.</t>
-  </si>
-  <si>
-    <t>Annexe 2</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Loi du 6 janvier 1978 relative à l'informatique, aux fichiers et aux libertés. Disponible sur </t>
     </r>
@@ -4137,141 +4125,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Recommandations aux commanditaires </t>
-    </r>
-  </si>
-  <si>
-    <t>a)     Le commanditaire peut, lorsqu’il est une autorité administrative ou un opérateur d’importance vitale, demander à l’ANSSI de participer à la définition du cahier des charges faisant l’objet d’un appel d’offres ou d’un contrat.</t>
-  </si>
-  <si>
-    <t>b)    Il est recommandé que le commanditaire choisisse son prestataire dans le catalogue des prestataires qualifiés publié sur le site de l’ANSSI, la qualification d’un prestataire d’informatique en nuage attestant de sa conformité à l’ensemble des exigences du présent référentiel.</t>
-  </si>
-  <si>
-    <t>c)     Pour bénéficier d’une prestation qualifiée, c’est-à-dire conforme à l’ensemble des exigences du présent référentiel, le commanditaire doit :</t>
-  </si>
-  <si>
-    <t>-        choisir le prestataire dans le catalogue des prestataires qualifiés publié sur le site de l’ANSSI ;</t>
-  </si>
-  <si>
-    <t>-        exiger du prestataire de stipuler dans la convention de service que la prestation réalisée est une prestation qualifiée.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">d)    Il est recommandé que le commanditaire utilise le guide d’achat des produits de sécurité et des services de confiance </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>[GUIDE_ACHAT]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> qui a pour vocation à accompagner la fonction achat des commanditaires lors des appels d’offres.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">e)     Le commanditaire peut, conformément au processus de qualification des prestataires de service de confiance </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>[PROCESS_QUALIF]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, déposer auprès de l’ANSSI une réclamation contre un prestataire qualifié pour lequel il estime que ce dernier n’a pas respecté une ou plusieurs exigences du présent référentiel dans le cadre d’une prestation qualifiée.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">f)      La qualification d’un prestataire n’atteste pas de sa capacité à accéder ou à détenir des informations classifiées de défense </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>[IGI_1300]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">g)     La qualification d’un prestataire n’atteste pas de sa capacité à accéder ou à détenir des articles contrôlés de la sécurité des systèmes d’information (ACSSI) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>[II_910]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">h)    La conformité du service du prestataire au référentiel SecNumCloud ne se substitue pas aux exigences légales ou réglementaires applicables à certaines données spécifiques telles que les données de niveau Diffusion Restreinte ou les données de santé. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">i)      Pour l’accès aux interfaces de gestion du service, il est recommandé que le commanditaire utilise des moyens (terminaux, serveurs) dédiés aux tâches d’administration et conformes aux recommandations du guide </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>[NT_ADMIN]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
 </sst>
@@ -4350,7 +4203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4358,53 +4211,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4876,10 +4723,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F3B91E-FB51-FE47-B7BA-EB94A985CF95}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E667"/>
+  <dimension ref="A1:E652"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A633" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D655" sqref="D655"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D656" sqref="D656"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5137,7 +4984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:5" ht="28" x14ac:dyDescent="0.15">
       <c r="B21" s="13">
         <v>4</v>
       </c>
@@ -5824,7 +5671,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B80" s="14">
+      <c r="B80" s="13">
         <v>2</v>
       </c>
       <c r="C80" s="7" t="s">
@@ -6052,7 +5899,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>5</v>
       </c>
@@ -6882,10 +6729,10 @@
       <c r="A165" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B165" s="15">
-        <v>3</v>
-      </c>
-      <c r="C165" s="16" t="s">
+      <c r="B165" s="14">
+        <v>3</v>
+      </c>
+      <c r="C165" s="15" t="s">
         <v>291</v>
       </c>
       <c r="E165" s="11" t="s">
@@ -6907,10 +6754,10 @@
       <c r="A167" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B167" s="15">
-        <v>3</v>
-      </c>
-      <c r="C167" s="16" t="s">
+      <c r="B167" s="14">
+        <v>3</v>
+      </c>
+      <c r="C167" s="15" t="s">
         <v>295</v>
       </c>
       <c r="E167" s="11" t="s">
@@ -6921,10 +6768,10 @@
       <c r="A168" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B168" s="15">
-        <v>3</v>
-      </c>
-      <c r="C168" s="16" t="s">
+      <c r="B168" s="14">
+        <v>3</v>
+      </c>
+      <c r="C168" s="15" t="s">
         <v>296</v>
       </c>
       <c r="E168" s="11" t="s">
@@ -6946,10 +6793,10 @@
       <c r="A170" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B170" s="15">
-        <v>3</v>
-      </c>
-      <c r="C170" s="16" t="s">
+      <c r="B170" s="14">
+        <v>3</v>
+      </c>
+      <c r="C170" s="15" t="s">
         <v>415</v>
       </c>
       <c r="E170" s="11" t="s">
@@ -6968,10 +6815,10 @@
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B172" s="15">
-        <v>3</v>
-      </c>
-      <c r="C172" s="16" t="s">
+      <c r="B172" s="14">
+        <v>3</v>
+      </c>
+      <c r="C172" s="15" t="s">
         <v>416</v>
       </c>
       <c r="E172" s="9"/>
@@ -7345,7 +7192,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A203" s="3" t="s">
         <v>5</v>
       </c>
@@ -7512,7 +7359,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A216" s="3" t="s">
         <v>5</v>
       </c>
@@ -7668,7 +7515,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="228" spans="1:5" ht="42" hidden="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:5" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A228" s="3" t="s">
         <v>5</v>
       </c>
@@ -7905,10 +7752,10 @@
       </c>
     </row>
     <row r="247" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B247" s="15">
+      <c r="B247" s="14">
         <v>2</v>
       </c>
-      <c r="C247" s="16" t="s">
+      <c r="C247" s="15" t="s">
         <v>444</v>
       </c>
       <c r="D247" s="9" t="s">
@@ -7972,10 +7819,10 @@
       </c>
     </row>
     <row r="252" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B252" s="15">
+      <c r="B252" s="14">
         <v>2</v>
       </c>
-      <c r="C252" s="16" t="s">
+      <c r="C252" s="15" t="s">
         <v>445</v>
       </c>
       <c r="D252" s="9" t="s">
@@ -8011,10 +7858,10 @@
       </c>
     </row>
     <row r="255" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B255" s="15">
+      <c r="B255" s="14">
         <v>2</v>
       </c>
-      <c r="C255" s="16" t="s">
+      <c r="C255" s="15" t="s">
         <v>446</v>
       </c>
       <c r="D255" s="9" t="s">
@@ -8078,10 +7925,10 @@
       </c>
     </row>
     <row r="260" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B260" s="15">
+      <c r="B260" s="14">
         <v>2</v>
       </c>
-      <c r="C260" s="16" t="s">
+      <c r="C260" s="15" t="s">
         <v>447</v>
       </c>
       <c r="D260" s="9" t="s">
@@ -8114,10 +7961,10 @@
       </c>
     </row>
     <row r="263" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B263" s="15">
+      <c r="B263" s="14">
         <v>2</v>
       </c>
-      <c r="C263" s="16" t="s">
+      <c r="C263" s="15" t="s">
         <v>448</v>
       </c>
       <c r="D263" s="9" t="s">
@@ -8258,10 +8105,10 @@
       </c>
     </row>
     <row r="275" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B275" s="15">
+      <c r="B275" s="14">
         <v>2</v>
       </c>
-      <c r="C275" s="16" t="s">
+      <c r="C275" s="15" t="s">
         <v>449</v>
       </c>
       <c r="D275" s="9" t="s">
@@ -8543,10 +8390,10 @@
       </c>
     </row>
     <row r="296" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B296" s="15">
+      <c r="B296" s="14">
         <v>2</v>
       </c>
-      <c r="C296" s="16" t="s">
+      <c r="C296" s="15" t="s">
         <v>450</v>
       </c>
       <c r="D296" s="9" t="s">
@@ -8624,17 +8471,17 @@
       </c>
     </row>
     <row r="302" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B302" s="15">
+      <c r="B302" s="14">
         <v>2</v>
       </c>
-      <c r="C302" s="16" t="s">
+      <c r="C302" s="15" t="s">
         <v>451</v>
       </c>
       <c r="D302" s="9" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="303" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A303" s="3" t="s">
         <v>5</v>
       </c>
@@ -8663,10 +8510,10 @@
       </c>
     </row>
     <row r="305" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B305" s="15">
+      <c r="B305" s="14">
         <v>2</v>
       </c>
-      <c r="C305" s="16" t="s">
+      <c r="C305" s="15" t="s">
         <v>452</v>
       </c>
       <c r="D305" s="9" t="s">
@@ -8702,10 +8549,10 @@
       </c>
     </row>
     <row r="308" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B308" s="15">
+      <c r="B308" s="14">
         <v>2</v>
       </c>
-      <c r="C308" s="16" t="s">
+      <c r="C308" s="15" t="s">
         <v>453</v>
       </c>
       <c r="D308" s="9" t="s">
@@ -8755,17 +8602,17 @@
       </c>
     </row>
     <row r="312" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B312" s="15">
+      <c r="B312" s="14">
         <v>2</v>
       </c>
-      <c r="C312" s="16" t="s">
+      <c r="C312" s="15" t="s">
         <v>454</v>
       </c>
       <c r="D312" s="9" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="313" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:5" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A313" s="3" t="s">
         <v>5</v>
       </c>
@@ -8822,10 +8669,10 @@
       </c>
     </row>
     <row r="317" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B317" s="15">
+      <c r="B317" s="14">
         <v>2</v>
       </c>
-      <c r="C317" s="16" t="s">
+      <c r="C317" s="15" t="s">
         <v>455</v>
       </c>
       <c r="D317" s="9" t="s">
@@ -8847,10 +8694,10 @@
       </c>
     </row>
     <row r="319" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B319" s="15">
+      <c r="B319" s="14">
         <v>2</v>
       </c>
-      <c r="C319" s="16" t="s">
+      <c r="C319" s="15" t="s">
         <v>456</v>
       </c>
       <c r="D319" s="9" t="s">
@@ -8872,10 +8719,10 @@
       </c>
     </row>
     <row r="321" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B321" s="15">
+      <c r="B321" s="14">
         <v>2</v>
       </c>
-      <c r="C321" s="16" t="s">
+      <c r="C321" s="15" t="s">
         <v>457</v>
       </c>
       <c r="D321" s="9" t="s">
@@ -9390,7 +9237,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="363" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:5" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A363" s="3" t="s">
         <v>5</v>
       </c>
@@ -9828,7 +9675,7 @@
       <c r="B397" s="12">
         <v>4</v>
       </c>
-      <c r="E397" s="19" t="s">
+      <c r="E397" s="17" t="s">
         <v>731</v>
       </c>
     </row>
@@ -9839,7 +9686,7 @@
       <c r="B398" s="12">
         <v>4</v>
       </c>
-      <c r="E398" s="19" t="s">
+      <c r="E398" s="17" t="s">
         <v>732</v>
       </c>
     </row>
@@ -9850,7 +9697,7 @@
       <c r="B399" s="12">
         <v>4</v>
       </c>
-      <c r="E399" s="19" t="s">
+      <c r="E399" s="17" t="s">
         <v>733</v>
       </c>
     </row>
@@ -9880,7 +9727,7 @@
       <c r="A402" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B402" s="18">
+      <c r="B402" s="12">
         <v>3</v>
       </c>
       <c r="C402" s="3" t="s">
@@ -9894,7 +9741,7 @@
       <c r="A403" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B403" s="18">
+      <c r="B403" s="12">
         <v>4</v>
       </c>
       <c r="C403" s="3"/>
@@ -9906,7 +9753,7 @@
       <c r="A404" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B404" s="18">
+      <c r="B404" s="12">
         <v>4</v>
       </c>
       <c r="E404" s="11" t="s">
@@ -9917,7 +9764,7 @@
       <c r="A405" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B405" s="18">
+      <c r="B405" s="12">
         <v>4</v>
       </c>
       <c r="E405" s="11" t="s">
@@ -9928,7 +9775,7 @@
       <c r="A406" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B406" s="18">
+      <c r="B406" s="12">
         <v>4</v>
       </c>
       <c r="E406" s="11" t="s">
@@ -9939,7 +9786,7 @@
       <c r="A407" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B407" s="18">
+      <c r="B407" s="12">
         <v>4</v>
       </c>
       <c r="E407" s="11" t="s">
@@ -9950,7 +9797,7 @@
       <c r="A408" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B408" s="18">
+      <c r="B408" s="12">
         <v>4</v>
       </c>
       <c r="E408" s="11" t="s">
@@ -9961,7 +9808,7 @@
       <c r="A409" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B409" s="18">
+      <c r="B409" s="12">
         <v>4</v>
       </c>
       <c r="E409" s="11" t="s">
@@ -9972,7 +9819,7 @@
       <c r="A410" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B410" s="18">
+      <c r="B410" s="12">
         <v>4</v>
       </c>
       <c r="E410" s="11" t="s">
@@ -9983,7 +9830,7 @@
       <c r="A411" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B411" s="18">
+      <c r="B411" s="12">
         <v>4</v>
       </c>
       <c r="E411" s="11" t="s">
@@ -9994,7 +9841,7 @@
       <c r="A412" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B412" s="18">
+      <c r="B412" s="12">
         <v>4</v>
       </c>
       <c r="E412" s="11" t="s">
@@ -10005,7 +9852,7 @@
       <c r="A413" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B413" s="18">
+      <c r="B413" s="12">
         <v>3</v>
       </c>
       <c r="C413" s="3" t="s">
@@ -10030,7 +9877,7 @@
       <c r="A415" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B415" s="18">
+      <c r="B415" s="12">
         <v>3</v>
       </c>
       <c r="C415" s="3" t="s">
@@ -10047,7 +9894,7 @@
       <c r="B416" s="12">
         <v>4</v>
       </c>
-      <c r="E416" s="17" t="s">
+      <c r="E416" s="16" t="s">
         <v>744</v>
       </c>
     </row>
@@ -10058,7 +9905,7 @@
       <c r="B417" s="12">
         <v>4</v>
       </c>
-      <c r="E417" s="17" t="s">
+      <c r="E417" s="16" t="s">
         <v>745</v>
       </c>
     </row>
@@ -10069,7 +9916,7 @@
       <c r="B418" s="12">
         <v>4</v>
       </c>
-      <c r="E418" s="17" t="s">
+      <c r="E418" s="16" t="s">
         <v>746</v>
       </c>
     </row>
@@ -10077,7 +9924,7 @@
       <c r="A419" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B419" s="18">
+      <c r="B419" s="12">
         <v>3</v>
       </c>
       <c r="C419" s="3" t="s">
@@ -10091,7 +9938,7 @@
       <c r="A420" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B420" s="18">
+      <c r="B420" s="12">
         <v>3</v>
       </c>
       <c r="C420" s="3" t="s">
@@ -10105,7 +9952,7 @@
       <c r="A421" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B421" s="18">
+      <c r="B421" s="12">
         <v>3</v>
       </c>
       <c r="C421" s="3" t="s">
@@ -10119,7 +9966,7 @@
       <c r="A422" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B422" s="18">
+      <c r="B422" s="12">
         <v>3</v>
       </c>
       <c r="C422" s="3" t="s">
@@ -10180,7 +10027,7 @@
       <c r="A427" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B427" s="18">
+      <c r="B427" s="12">
         <v>3</v>
       </c>
       <c r="C427" s="3" t="s">
@@ -10194,7 +10041,7 @@
       <c r="A428" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B428" s="18">
+      <c r="B428" s="12">
         <v>3</v>
       </c>
       <c r="C428" s="3" t="s">
@@ -10219,7 +10066,7 @@
       <c r="A430" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B430" s="18">
+      <c r="B430" s="12">
         <v>3</v>
       </c>
       <c r="C430" s="3" t="s">
@@ -10233,7 +10080,7 @@
       <c r="A431" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B431" s="18">
+      <c r="B431" s="12">
         <v>3</v>
       </c>
       <c r="C431" s="3" t="s">
@@ -10247,7 +10094,7 @@
       <c r="A432" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B432" s="18">
+      <c r="B432" s="12">
         <v>3</v>
       </c>
       <c r="C432" s="3" t="s">
@@ -10272,7 +10119,7 @@
       <c r="A434" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B434" s="18">
+      <c r="B434" s="12">
         <v>3</v>
       </c>
       <c r="C434" s="3" t="s">
@@ -10297,7 +10144,7 @@
       <c r="A436" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B436" s="18">
+      <c r="B436" s="12">
         <v>3</v>
       </c>
       <c r="C436" s="3" t="s">
@@ -10311,7 +10158,7 @@
       <c r="A437" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B437" s="18">
+      <c r="B437" s="12">
         <v>3</v>
       </c>
       <c r="C437" s="3" t="s">
@@ -10336,7 +10183,7 @@
       <c r="A439" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B439" s="18">
+      <c r="B439" s="12">
         <v>3</v>
       </c>
       <c r="C439" s="3" t="s">
@@ -10361,7 +10208,7 @@
       <c r="A441" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B441" s="18">
+      <c r="B441" s="12">
         <v>3</v>
       </c>
       <c r="C441" s="3" t="s">
@@ -10408,7 +10255,7 @@
       <c r="A445" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B445" s="18">
+      <c r="B445" s="12">
         <v>3</v>
       </c>
       <c r="C445" s="3" t="s">
@@ -10422,7 +10269,7 @@
       <c r="A446" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B446" s="18">
+      <c r="B446" s="12">
         <v>3</v>
       </c>
       <c r="C446" s="3" t="s">
@@ -10458,7 +10305,7 @@
       <c r="A449" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B449" s="18">
+      <c r="B449" s="12">
         <v>3</v>
       </c>
       <c r="C449" s="3" t="s">
@@ -10472,7 +10319,7 @@
       <c r="A450" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B450" s="18">
+      <c r="B450" s="12">
         <v>3</v>
       </c>
       <c r="C450" s="3" t="s">
@@ -10497,7 +10344,7 @@
       <c r="A452" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B452" s="18">
+      <c r="B452" s="12">
         <v>3</v>
       </c>
       <c r="C452" s="3" t="s">
@@ -10511,7 +10358,7 @@
       <c r="A453" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B453" s="18">
+      <c r="B453" s="12">
         <v>3</v>
       </c>
       <c r="C453" s="3" t="s">
@@ -10525,7 +10372,7 @@
       <c r="A454" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B454" s="18">
+      <c r="B454" s="12">
         <v>3</v>
       </c>
       <c r="C454" s="3" t="s">
@@ -10550,7 +10397,7 @@
       <c r="A456" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B456" s="18">
+      <c r="B456" s="12">
         <v>3</v>
       </c>
       <c r="C456" s="3" t="s">
@@ -10575,7 +10422,7 @@
       <c r="A458" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B458" s="18">
+      <c r="B458" s="12">
         <v>3</v>
       </c>
       <c r="C458" s="3" t="s">
@@ -10589,7 +10436,7 @@
       <c r="A459" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B459" s="18">
+      <c r="B459" s="12">
         <v>3</v>
       </c>
       <c r="C459" s="3" t="s">
@@ -10614,7 +10461,7 @@
       <c r="A461" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B461" s="18">
+      <c r="B461" s="12">
         <v>3</v>
       </c>
       <c r="C461" s="3" t="s">
@@ -10650,7 +10497,7 @@
       <c r="A464" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B464" s="18">
+      <c r="B464" s="12">
         <v>3</v>
       </c>
       <c r="C464" s="3" t="s">
@@ -10664,7 +10511,7 @@
       <c r="A465" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B465" s="18">
+      <c r="B465" s="12">
         <v>3</v>
       </c>
       <c r="C465" s="3" t="s">
@@ -10678,7 +10525,7 @@
       <c r="A466" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B466" s="18">
+      <c r="B466" s="12">
         <v>3</v>
       </c>
       <c r="C466" s="3" t="s">
@@ -10703,7 +10550,7 @@
       <c r="A468" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B468" s="18">
+      <c r="B468" s="12">
         <v>3</v>
       </c>
       <c r="C468" s="3" t="s">
@@ -10717,7 +10564,7 @@
       <c r="A469" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B469" s="18">
+      <c r="B469" s="12">
         <v>3</v>
       </c>
       <c r="C469" s="3" t="s">
@@ -10731,7 +10578,7 @@
       <c r="A470" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B470" s="18">
+      <c r="B470" s="12">
         <v>3</v>
       </c>
       <c r="C470" s="3" t="s">
@@ -10745,7 +10592,7 @@
       <c r="A471" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B471" s="18">
+      <c r="B471" s="12">
         <v>3</v>
       </c>
       <c r="C471" s="3" t="s">
@@ -10770,7 +10617,7 @@
       <c r="A473" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B473" s="18">
+      <c r="B473" s="12">
         <v>3</v>
       </c>
       <c r="C473" s="3" t="s">
@@ -10784,7 +10631,7 @@
       <c r="A474" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B474" s="18">
+      <c r="B474" s="12">
         <v>3</v>
       </c>
       <c r="C474" s="3" t="s">
@@ -10809,7 +10656,7 @@
       <c r="A476" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B476" s="18">
+      <c r="B476" s="12">
         <v>3</v>
       </c>
       <c r="C476" s="3" t="s">
@@ -10823,7 +10670,7 @@
       <c r="A477" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B477" s="18">
+      <c r="B477" s="12">
         <v>3</v>
       </c>
       <c r="C477" s="3" t="s">
@@ -10837,7 +10684,7 @@
       <c r="A478" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B478" s="18">
+      <c r="B478" s="12">
         <v>3</v>
       </c>
       <c r="C478" s="3" t="s">
@@ -10862,7 +10709,7 @@
       <c r="A480" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B480" s="18">
+      <c r="B480" s="12">
         <v>3</v>
       </c>
       <c r="C480" s="3" t="s">
@@ -10887,7 +10734,7 @@
       <c r="A482" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B482" s="18">
+      <c r="B482" s="12">
         <v>3</v>
       </c>
       <c r="C482" s="3" t="s">
@@ -10923,7 +10770,7 @@
       <c r="A485" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B485" s="18">
+      <c r="B485" s="12">
         <v>3</v>
       </c>
       <c r="C485" s="3" t="s">
@@ -10937,7 +10784,7 @@
       <c r="A486" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B486" s="18">
+      <c r="B486" s="12">
         <v>3</v>
       </c>
       <c r="C486" s="3" t="s">
@@ -10962,7 +10809,7 @@
       <c r="A488" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B488" s="18">
+      <c r="B488" s="12">
         <v>3</v>
       </c>
       <c r="C488" s="3" t="s">
@@ -10987,7 +10834,7 @@
       <c r="A490" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B490" s="18">
+      <c r="B490" s="12">
         <v>3</v>
       </c>
       <c r="C490" s="3" t="s">
@@ -11008,11 +10855,11 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="492" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="492" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A492" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B492" s="18">
+      <c r="B492" s="12">
         <v>3</v>
       </c>
       <c r="C492" s="3" t="s">
@@ -11037,7 +10884,7 @@
       <c r="A494" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B494" s="18">
+      <c r="B494" s="12">
         <v>3</v>
       </c>
       <c r="C494" s="3" t="s">
@@ -11062,7 +10909,7 @@
       <c r="A496" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B496" s="18">
+      <c r="B496" s="12">
         <v>3</v>
       </c>
       <c r="C496" s="3" t="s">
@@ -11098,7 +10945,7 @@
       <c r="A499" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B499" s="18">
+      <c r="B499" s="12">
         <v>3</v>
       </c>
       <c r="C499" s="3" t="s">
@@ -11112,7 +10959,7 @@
       <c r="A500" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B500" s="18">
+      <c r="B500" s="12">
         <v>4</v>
       </c>
       <c r="C500" s="3"/>
@@ -11124,7 +10971,7 @@
       <c r="A501" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B501" s="18">
+      <c r="B501" s="12">
         <v>4</v>
       </c>
       <c r="C501" s="3"/>
@@ -11136,7 +10983,7 @@
       <c r="A502" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B502" s="18">
+      <c r="B502" s="12">
         <v>4</v>
       </c>
       <c r="E502" s="11" t="s">
@@ -11147,7 +10994,7 @@
       <c r="A503" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B503" s="18">
+      <c r="B503" s="12">
         <v>4</v>
       </c>
       <c r="E503" s="11" t="s">
@@ -11158,7 +11005,7 @@
       <c r="A504" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B504" s="18">
+      <c r="B504" s="12">
         <v>4</v>
       </c>
       <c r="E504" s="11" t="s">
@@ -11169,7 +11016,7 @@
       <c r="A505" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B505" s="18">
+      <c r="B505" s="12">
         <v>4</v>
       </c>
       <c r="E505" s="11" t="s">
@@ -11180,7 +11027,7 @@
       <c r="A506" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B506" s="18">
+      <c r="B506" s="12">
         <v>3</v>
       </c>
       <c r="C506" s="3" t="s">
@@ -11194,7 +11041,7 @@
       <c r="A507" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B507" s="18">
+      <c r="B507" s="12">
         <v>3</v>
       </c>
       <c r="C507" s="3" t="s">
@@ -11208,7 +11055,7 @@
       <c r="A508" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B508" s="18">
+      <c r="B508" s="12">
         <v>3</v>
       </c>
       <c r="C508" s="3" t="s">
@@ -11222,7 +11069,7 @@
       <c r="A509" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B509" s="18">
+      <c r="B509" s="12">
         <v>3</v>
       </c>
       <c r="C509" s="3" t="s">
@@ -11244,7 +11091,7 @@
       </c>
     </row>
     <row r="511" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B511" s="18">
+      <c r="B511" s="12">
         <v>3</v>
       </c>
       <c r="C511" s="3" t="s">
@@ -11255,7 +11102,7 @@
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B512" s="18">
+      <c r="B512" s="12">
         <v>4</v>
       </c>
       <c r="C512" s="3" t="s">
@@ -11267,7 +11114,7 @@
       <c r="A513" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B513" s="18">
+      <c r="B513" s="12">
         <v>5</v>
       </c>
       <c r="C513" s="3"/>
@@ -11334,7 +11181,7 @@
       <c r="A519" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B519" s="18">
+      <c r="B519" s="12">
         <v>4</v>
       </c>
       <c r="C519" s="3" t="s">
@@ -11497,7 +11344,7 @@
       <c r="A533" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B533" s="18">
+      <c r="B533" s="12">
         <v>3</v>
       </c>
       <c r="C533" s="3" t="s">
@@ -11558,7 +11405,7 @@
       <c r="A538" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B538" s="18">
+      <c r="B538" s="12">
         <v>3</v>
       </c>
       <c r="C538" s="3" t="s">
@@ -11572,7 +11419,7 @@
       <c r="A539" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B539" s="18">
+      <c r="B539" s="12">
         <v>3</v>
       </c>
       <c r="C539" s="3" t="s">
@@ -11586,7 +11433,7 @@
       <c r="A540" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B540" s="18">
+      <c r="B540" s="12">
         <v>4</v>
       </c>
       <c r="C540" s="3"/>
@@ -11598,7 +11445,7 @@
       <c r="A541" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B541" s="18">
+      <c r="B541" s="12">
         <v>4</v>
       </c>
       <c r="C541" s="3"/>
@@ -11610,7 +11457,7 @@
       <c r="A542" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B542" s="18">
+      <c r="B542" s="12">
         <v>4</v>
       </c>
       <c r="C542" s="3"/>
@@ -11622,7 +11469,7 @@
       <c r="A543" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B543" s="18">
+      <c r="B543" s="12">
         <v>3</v>
       </c>
       <c r="C543" s="3" t="s">
@@ -11636,7 +11483,7 @@
       <c r="A544" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B544" s="18">
+      <c r="B544" s="12">
         <v>3</v>
       </c>
       <c r="C544" s="3" t="s">
@@ -11650,7 +11497,7 @@
       <c r="A545" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B545" s="18">
+      <c r="B545" s="12">
         <v>3</v>
       </c>
       <c r="C545" s="3" t="s">
@@ -11664,7 +11511,7 @@
       <c r="A546" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B546" s="18">
+      <c r="B546" s="12">
         <v>3</v>
       </c>
       <c r="C546" s="3" t="s">
@@ -11678,7 +11525,7 @@
       <c r="A547" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B547" s="18">
+      <c r="B547" s="12">
         <v>3</v>
       </c>
       <c r="C547" s="3" t="s">
@@ -11692,7 +11539,7 @@
       <c r="A548" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B548" s="18">
+      <c r="B548" s="12">
         <v>3</v>
       </c>
       <c r="C548" s="3" t="s">
@@ -11706,7 +11553,7 @@
       <c r="A549" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B549" s="18">
+      <c r="B549" s="12">
         <v>3</v>
       </c>
       <c r="C549" s="3" t="s">
@@ -11753,7 +11600,7 @@
       <c r="A553" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B553" s="18">
+      <c r="B553" s="12">
         <v>3</v>
       </c>
       <c r="C553" s="3" t="s">
@@ -11763,11 +11610,11 @@
         <v>949</v>
       </c>
     </row>
-    <row r="554" spans="1:5" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="554" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A554" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B554" s="18">
+      <c r="B554" s="12">
         <v>3</v>
       </c>
       <c r="C554" s="3" t="s">
@@ -11781,7 +11628,7 @@
       <c r="A555" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B555" s="18">
+      <c r="B555" s="12">
         <v>3</v>
       </c>
       <c r="C555" s="3" t="s">
@@ -11795,7 +11642,7 @@
       <c r="A556" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B556" s="18">
+      <c r="B556" s="12">
         <v>3</v>
       </c>
       <c r="C556" s="3" t="s">
@@ -11809,7 +11656,7 @@
       <c r="A557" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B557" s="18">
+      <c r="B557" s="12">
         <v>3</v>
       </c>
       <c r="C557" s="3" t="s">
@@ -11823,7 +11670,7 @@
       <c r="A558" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B558" s="18">
+      <c r="B558" s="12">
         <v>3</v>
       </c>
       <c r="C558" s="3" t="s">
@@ -11870,7 +11717,7 @@
       <c r="A562" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B562" s="18">
+      <c r="B562" s="12">
         <v>3</v>
       </c>
       <c r="C562" s="3" t="s">
@@ -11884,7 +11731,7 @@
       <c r="A563" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B563" s="18">
+      <c r="B563" s="12">
         <v>3</v>
       </c>
       <c r="C563" s="3" t="s">
@@ -11898,7 +11745,7 @@
       <c r="A564" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B564" s="18">
+      <c r="B564" s="12">
         <v>3</v>
       </c>
       <c r="C564" s="3" t="s">
@@ -11923,7 +11770,7 @@
       <c r="A566" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B566" s="18">
+      <c r="B566" s="12">
         <v>3</v>
       </c>
       <c r="C566" s="3" t="s">
@@ -11937,7 +11784,7 @@
       <c r="A567" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B567" s="18">
+      <c r="B567" s="12">
         <v>3</v>
       </c>
       <c r="C567" s="3" t="s">
@@ -11951,7 +11798,7 @@
       <c r="A568" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B568" s="18">
+      <c r="B568" s="12">
         <v>3</v>
       </c>
       <c r="C568" s="3" t="s">
@@ -11965,7 +11812,7 @@
       <c r="A569" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B569" s="18">
+      <c r="B569" s="12">
         <v>3</v>
       </c>
       <c r="C569" s="3" t="s">
@@ -11975,11 +11822,11 @@
         <v>923</v>
       </c>
     </row>
-    <row r="570" spans="1:5" ht="28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="570" spans="1:5" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A570" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B570" s="18">
+      <c r="B570" s="12">
         <v>3</v>
       </c>
       <c r="C570" s="3" t="s">
@@ -12004,7 +11851,7 @@
       <c r="A572" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B572" s="18">
+      <c r="B572" s="12">
         <v>3</v>
       </c>
       <c r="C572" s="3" t="s">
@@ -12018,7 +11865,7 @@
       <c r="A573" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B573" s="18">
+      <c r="B573" s="12">
         <v>3</v>
       </c>
       <c r="C573" s="3" t="s">
@@ -12043,7 +11890,7 @@
       <c r="A575" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B575" s="18">
+      <c r="B575" s="12">
         <v>3</v>
       </c>
       <c r="C575" s="3" t="s">
@@ -12057,7 +11904,7 @@
       <c r="A576" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B576" s="18">
+      <c r="B576" s="12">
         <v>4</v>
       </c>
       <c r="C576" s="3"/>
@@ -12091,7 +11938,7 @@
       <c r="A579" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B579" s="18">
+      <c r="B579" s="12">
         <v>3</v>
       </c>
       <c r="C579" s="3" t="s">
@@ -12116,7 +11963,7 @@
       <c r="A581" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B581" s="18">
+      <c r="B581" s="12">
         <v>3</v>
       </c>
       <c r="C581" s="3" t="s">
@@ -12207,7 +12054,7 @@
       <c r="A589" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B589" s="18">
+      <c r="B589" s="12">
         <v>3</v>
       </c>
       <c r="C589" s="3" t="s">
@@ -12265,7 +12112,7 @@
       <c r="A594" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B594" s="18">
+      <c r="B594" s="12">
         <v>3</v>
       </c>
       <c r="C594" s="3" t="s">
@@ -12290,7 +12137,7 @@
       <c r="A596" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B596" s="18">
+      <c r="B596" s="12">
         <v>3</v>
       </c>
       <c r="C596" s="3" t="s">
@@ -12301,7 +12148,7 @@
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B597" s="18">
+      <c r="B597" s="12">
         <v>3</v>
       </c>
       <c r="C597" s="3" t="s">
@@ -12313,7 +12160,7 @@
       <c r="A598" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B598" s="18">
+      <c r="B598" s="12">
         <v>4</v>
       </c>
       <c r="C598" s="3"/>
@@ -12388,7 +12235,7 @@
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B605" s="18">
+      <c r="B605" s="12">
         <v>3</v>
       </c>
       <c r="C605" s="3" t="s">
@@ -12400,7 +12247,7 @@
       <c r="A606" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B606" s="18">
+      <c r="B606" s="12">
         <v>4</v>
       </c>
       <c r="C606" s="3"/>
@@ -12420,7 +12267,7 @@
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B608" s="18">
+      <c r="B608" s="12">
         <v>3</v>
       </c>
       <c r="C608" s="3" t="s">
@@ -12455,7 +12302,7 @@
       <c r="A611" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B611" s="18">
+      <c r="B611" s="12">
         <v>3</v>
       </c>
       <c r="C611" s="3" t="s">
@@ -12469,7 +12316,7 @@
       <c r="A612" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B612" s="18">
+      <c r="B612" s="12">
         <v>3</v>
       </c>
       <c r="C612" s="3" t="s">
@@ -12494,10 +12341,10 @@
       <c r="B614" s="12">
         <v>2</v>
       </c>
-      <c r="C614" s="20" t="s">
+      <c r="C614" s="18" t="s">
         <v>1076</v>
       </c>
-      <c r="D614" s="20" t="s">
+      <c r="D614" s="18" t="s">
         <v>1075</v>
       </c>
     </row>
@@ -12509,14 +12356,14 @@
         <v>1077</v>
       </c>
       <c r="E615" s="11" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="616" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="B616" s="12">
         <v>3</v>
       </c>
-      <c r="D616" s="21" t="s">
+      <c r="D616" s="19" t="s">
         <v>1078</v>
       </c>
       <c r="E616" s="11" t="s">
@@ -12527,9 +12374,9 @@
       <c r="B617" s="12">
         <v>3</v>
       </c>
-      <c r="D617" s="21"/>
+      <c r="D617" s="19"/>
       <c r="E617" s="10" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="618" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -12540,7 +12387,7 @@
         <v>1080</v>
       </c>
       <c r="E618" s="11" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="619" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -12551,7 +12398,7 @@
         <v>1081</v>
       </c>
       <c r="E619" s="11" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="620" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -12562,7 +12409,7 @@
         <v>1082</v>
       </c>
       <c r="E620" s="11" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="621" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -12573,7 +12420,7 @@
         <v>1083</v>
       </c>
       <c r="E621" s="11" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="622" spans="1:5" ht="14" x14ac:dyDescent="0.15">
@@ -12584,34 +12431,34 @@
         <v>1084</v>
       </c>
       <c r="E622" s="10" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="623" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="B623" s="12">
         <v>3</v>
       </c>
-      <c r="D623" s="21" t="s">
+      <c r="D623" s="19" t="s">
         <v>1085</v>
       </c>
       <c r="E623" s="10" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="624" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="B624" s="12">
         <v>3</v>
       </c>
-      <c r="D624" s="21"/>
+      <c r="D624" s="19"/>
       <c r="E624" s="10" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="625" spans="2:5" ht="14" x14ac:dyDescent="0.15">
       <c r="B625" s="12">
         <v>3</v>
       </c>
-      <c r="D625" s="21" t="s">
+      <c r="D625" s="19" t="s">
         <v>1086</v>
       </c>
       <c r="E625" s="11" t="s">
@@ -12622,9 +12469,9 @@
       <c r="B626" s="12">
         <v>3</v>
       </c>
-      <c r="D626" s="21"/>
+      <c r="D626" s="19"/>
       <c r="E626" s="10" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="627" spans="2:5" ht="28" x14ac:dyDescent="0.15">
@@ -12635,7 +12482,7 @@
         <v>1088</v>
       </c>
       <c r="E627" s="11" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="628" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12668,7 +12515,7 @@
         <v>1093</v>
       </c>
       <c r="E630" s="11" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="631" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12701,7 +12548,7 @@
         <v>1098</v>
       </c>
       <c r="E633" s="11" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="634" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12745,7 +12592,7 @@
         <v>1105</v>
       </c>
       <c r="E637" s="11" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="638" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12767,14 +12614,14 @@
         <v>1108</v>
       </c>
       <c r="E639" s="11" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="640" spans="2:5" ht="14" x14ac:dyDescent="0.15">
       <c r="B640" s="12">
         <v>3</v>
       </c>
-      <c r="D640" s="21" t="s">
+      <c r="D640" s="19" t="s">
         <v>1109</v>
       </c>
       <c r="E640" s="11" t="s">
@@ -12785,9 +12632,9 @@
       <c r="B641" s="12">
         <v>3</v>
       </c>
-      <c r="D641" s="21"/>
+      <c r="D641" s="19"/>
       <c r="E641" s="11" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="642" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12809,7 +12656,7 @@
         <v>1113</v>
       </c>
       <c r="E643" s="11" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="644" spans="2:5" ht="28" x14ac:dyDescent="0.15">
@@ -12820,7 +12667,7 @@
         <v>1114</v>
       </c>
       <c r="E644" s="11" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="645" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12831,7 +12678,7 @@
         <v>1115</v>
       </c>
       <c r="E645" s="10" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="646" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12842,7 +12689,7 @@
         <v>1116</v>
       </c>
       <c r="E646" s="11" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="647" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12853,7 +12700,7 @@
         <v>1117</v>
       </c>
       <c r="E647" s="10" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="648" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12874,7 +12721,7 @@
       <c r="C649" s="7" t="s">
         <v>1121</v>
       </c>
-      <c r="D649" s="20" t="s">
+      <c r="D649" s="18" t="s">
         <v>1120</v>
       </c>
     </row>
@@ -12886,7 +12733,7 @@
         <v>1122</v>
       </c>
       <c r="E650" s="11" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="651" spans="2:5" ht="14" x14ac:dyDescent="0.15">
@@ -12909,131 +12756,6 @@
       </c>
       <c r="E652" s="11" t="s">
         <v>1126</v>
-      </c>
-    </row>
-    <row r="653" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B653" s="12">
-        <v>1</v>
-      </c>
-      <c r="C653" s="7" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D653" s="7" t="s">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="654" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B654" s="12">
-        <v>2</v>
-      </c>
-      <c r="D654" s="3"/>
-      <c r="E654" s="11" t="s">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="655" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B655" s="12">
-        <v>2</v>
-      </c>
-      <c r="D655" s="3"/>
-      <c r="E655" s="11" t="s">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="656" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B656" s="12">
-        <v>2</v>
-      </c>
-      <c r="E656" s="11" t="s">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="657" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B657" s="12">
-        <v>2</v>
-      </c>
-      <c r="E657" s="11" t="s">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="658" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B658" s="12">
-        <v>3</v>
-      </c>
-      <c r="E658" s="11" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="659" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B659" s="12">
-        <v>3</v>
-      </c>
-      <c r="E659" s="11" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="660" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B660" s="12">
-        <v>2</v>
-      </c>
-      <c r="E660" s="11" t="s">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="661" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B661" s="12">
-        <v>2</v>
-      </c>
-      <c r="E661" s="11" t="s">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="662" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B662" s="12">
-        <v>2</v>
-      </c>
-      <c r="E662" s="11" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="663" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B663" s="12">
-        <v>2</v>
-      </c>
-      <c r="E663" s="11" t="s">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="664" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B664" s="12">
-        <v>2</v>
-      </c>
-      <c r="E664" s="11" t="s">
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="665" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B665" s="12">
-        <v>2</v>
-      </c>
-      <c r="E665" s="11" t="s">
-        <v>1161</v>
-      </c>
-    </row>
-    <row r="666" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B666" s="12">
-        <v>2</v>
-      </c>
-      <c r="E666" s="11" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="667" spans="2:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="B667" s="12">
-        <v>2</v>
-      </c>
-      <c r="E667" s="11" t="s">
-        <v>1163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>